<commit_message>
feat: Liquidar cuando se crean guias desde excel
</commit_message>
<xml_diff>
--- a/public/estructura/estructuraGenerarGuia.xlsx
+++ b/public/estructura/estructuraGenerarGuia.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">fecha</t>
   </si>
   <si>
-    <t xml:space="preserve">Aaaa-mm-dd hh:mm:ss</t>
+    <t xml:space="preserve">aaaa-mm-dd hh:mm:ss</t>
   </si>
   <si>
     <t xml:space="preserve">IMPORTANTE</t>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t xml:space="preserve">comentario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tipo_liquidacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indica el lipo de liquidacion y acepta solo los siguientes valores (K=kilo, U=unidad, A=adicional)</t>
   </si>
 </sst>
 </file>
@@ -253,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -276,6 +282,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -355,10 +365,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J34" activeCellId="0" sqref="J34"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -875,7 +885,32 @@
         <v>7</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F31:J31"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
feat: Ajustes al formato de despacho se agregan comentarios y la ruta del despacho.
_Se agregan los archivos ejemplo de excel de guias y la estructura informativa
</commit_message>
<xml_diff>
--- a/public/estructura/estructuraGenerarGuia.xlsx
+++ b/public/estructura/estructuraGenerarGuia.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">obligatorio</t>
   </si>
   <si>
-    <t xml:space="preserve">codigo_guia_tipo_fk</t>
+    <t xml:space="preserve">codigo_ciudad_destino_fk</t>
   </si>
   <si>
     <t xml:space="preserve">texto</t>
@@ -46,112 +46,40 @@
     <t xml:space="preserve">si</t>
   </si>
   <si>
-    <t xml:space="preserve">codigo_operacion_ingreso_fk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">codigo_operacion_cargo_fk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">codigo_cliente_fk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">codigo_ciudad_origen_fk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">codigo_ciudad_destino_fk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">codigo_servicio_fk</t>
-  </si>
-  <si>
     <t xml:space="preserve">codigo_producto_fk</t>
   </si>
   <si>
-    <t xml:space="preserve">codigo_empaque_fk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">codigo_condicion_fk</t>
+    <t xml:space="preserve">documento_cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre_destinatario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direccion_destinatario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">telefono_destinatario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unidades</t>
   </si>
   <si>
     <t xml:space="preserve">flotante</t>
   </si>
   <si>
-    <t xml:space="preserve">documento_cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relacion_cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remitente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nombre_destinatario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">direccion_destinatario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">telefono_destinatario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fecha_ingreso</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fecha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aaaa-mm-dd hh:mm:ss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPORTANTE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agregar al final del dato fecha_ingreso una comilla doble, asi 2019-01-01 12:24:12”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unidades</t>
-  </si>
-  <si>
     <t xml:space="preserve">peso_real</t>
   </si>
   <si>
     <t xml:space="preserve">peso_volumen</t>
   </si>
   <si>
-    <t xml:space="preserve">peso_facturado</t>
-  </si>
-  <si>
     <t xml:space="preserve">vr_declara</t>
   </si>
   <si>
-    <t xml:space="preserve">vr_flete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vr_manejo</t>
-  </si>
-  <si>
     <t xml:space="preserve">vr_recaudo</t>
   </si>
   <si>
-    <t xml:space="preserve">mercancia_peligrosa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boleano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usuario</t>
-  </si>
-  <si>
     <t xml:space="preserve">comentario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tipo_liquidacion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indica el lipo de liquidacion y acepta solo los siguientes valores (K=kilo, U=unidad, A=adicional)</t>
   </si>
 </sst>
 </file>
@@ -161,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -192,13 +120,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -259,7 +180,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -278,14 +199,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -365,10 +278,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -476,7 +389,6 @@
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -492,7 +404,6 @@
       <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -503,36 +414,37 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="n">
+        <v>150</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="n">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>7</v>
@@ -540,14 +452,14 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="n">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>7</v>
@@ -555,15 +467,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4" t="n">
-        <v>20</v>
-      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
@@ -573,12 +483,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="4" t="n">
-        <v>20</v>
-      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
@@ -588,12 +496,10 @@
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="4" t="n">
-        <v>20</v>
-      </c>
+      <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
         <v>7</v>
       </c>
@@ -603,7 +509,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -613,10 +519,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -633,284 +539,13 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="n">
-        <v>80</v>
+        <v>2000</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="n">
-        <v>50</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4" t="n">
-        <v>80</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="n">
-        <v>150</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4" t="n">
-        <v>150</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4" t="n">
-        <v>80</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4" t="n">
-        <v>25</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F31:J31"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Cambios en el archivo de importar
</commit_message>
<xml_diff>
--- a/public/estructura/estructuraGenerarGuia.xlsx
+++ b/public/estructura/estructuraGenerarGuia.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">documento_cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relacion_cliente</t>
   </si>
   <si>
     <t xml:space="preserve">nombre_destinatario</t>
@@ -278,10 +281,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -429,7 +432,7 @@
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>7</v>
@@ -459,7 +462,7 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>7</v>
@@ -470,20 +473,22 @@
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4" t="n">
+        <v>80</v>
+      </c>
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -496,7 +501,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -509,7 +514,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -522,7 +527,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -535,13 +540,26 @@
         <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="4" t="n">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="n">
         <v>2000</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>